<commit_message>
Update file register and Login/loginAdmin and add Revise In Excel
</commit_message>
<xml_diff>
--- a/ExcelProject/Login.xlsx
+++ b/ExcelProject/Login.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jalem\OneDrive\Desktop\Project100%\ExcelProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jalem\OneDrive\Desktop\Project_Test_Tutors\ExcelProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59DFDEE2-8036-43AE-950C-43ABBBA127F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0753B321-5463-4FE2-877F-8A1AB7B6DBDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="58">
   <si>
     <t>TestCase</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>ActualResult</t>
+  </si>
+  <si>
+    <t>Revise</t>
   </si>
 </sst>
 </file>
@@ -287,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -300,10 +303,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
@@ -587,7 +586,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -622,7 +621,9 @@
       <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="8"/>
+      <c r="H1" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
@@ -642,7 +643,7 @@
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="9"/>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
@@ -662,7 +663,7 @@
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="9"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
@@ -682,7 +683,7 @@
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="9"/>
+      <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
@@ -702,7 +703,7 @@
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="9"/>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
@@ -722,7 +723,7 @@
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="9"/>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
@@ -742,7 +743,7 @@
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="9"/>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
@@ -762,7 +763,7 @@
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="9"/>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
@@ -780,7 +781,7 @@
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="9"/>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
@@ -800,7 +801,7 @@
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="9"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
@@ -820,7 +821,7 @@
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="9"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
@@ -840,7 +841,7 @@
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="9"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
@@ -860,7 +861,7 @@
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="9"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
@@ -880,7 +881,7 @@
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="9"/>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
@@ -900,7 +901,7 @@
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="9"/>
+      <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
@@ -920,7 +921,7 @@
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="9"/>
+      <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
@@ -940,7 +941,7 @@
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="9"/>
+      <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
@@ -960,7 +961,7 @@
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="9"/>
+      <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
@@ -980,7 +981,7 @@
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
-      <c r="H19" s="9"/>
+      <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
@@ -1000,7 +1001,7 @@
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
-      <c r="H20" s="9"/>
+      <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
@@ -1020,7 +1021,7 @@
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="9"/>
+      <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
@@ -1038,7 +1039,7 @@
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="9"/>
+      <c r="H22" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Add Test Register Tutor
</commit_message>
<xml_diff>
--- a/ExcelProject/Login.xlsx
+++ b/ExcelProject/Login.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jalem\OneDrive\Desktop\Project_Test_Tutors\ExcelProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342DD402-8AA1-484D-ACDC-B1254C350244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5E6C9E-5EBA-4F86-9590-396661D9691F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11925" yWindow="3360" windowWidth="14610" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="71">
   <si>
     <t>Execute</t>
   </si>
@@ -58,177 +58,159 @@
     <t>Ptt123445678##</t>
   </si>
   <si>
-    <t>เข้าสู่ระบบสำเร็จ</t>
-  </si>
-  <si>
     <t>เข้าสู่ระบบเรียบร้อย</t>
   </si>
   <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>TC3:02</t>
+  </si>
+  <si>
+    <t>pattrawut</t>
+  </si>
+  <si>
+    <t>ความยาวรหัสนักศึกษาต้องมี 13 ตัวพอดี</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>TC3:03</t>
+  </si>
+  <si>
+    <t>MJU6504106337</t>
+  </si>
+  <si>
+    <t>TC3:04</t>
+  </si>
+  <si>
+    <t>MJU 650410640</t>
+  </si>
+  <si>
+    <t>กรุณากรอกข้อมูลอีเมล์และรหัสผ่านโดยห้ามมีช่องว่าง</t>
+  </si>
+  <si>
+    <t>TC3:05</t>
+  </si>
+  <si>
+    <t>mju6504106400</t>
+  </si>
+  <si>
+    <t>TC3:06</t>
+  </si>
+  <si>
+    <t>mju650410640</t>
+  </si>
+  <si>
+    <t>TC3:07</t>
+  </si>
+  <si>
+    <t>mju65041064001</t>
+  </si>
+  <si>
+    <t>TC3:08</t>
+  </si>
+  <si>
+    <t>กรุณากรอกรหัสนักศึกษาและรหัสผ่าน</t>
+  </si>
+  <si>
+    <t>TC3:09</t>
+  </si>
+  <si>
+    <t>MJU6504106436</t>
+  </si>
+  <si>
+    <t>TC3:10</t>
+  </si>
+  <si>
+    <t>MJU6504106437</t>
+  </si>
+  <si>
+    <t>รหัสผ่าน</t>
+  </si>
+  <si>
+    <t>ชื่อผู้ใช้หรือรหัสผ่านไม่ถูกต้อง</t>
+  </si>
+  <si>
+    <t>TC3:11</t>
+  </si>
+  <si>
+    <t>MJU6504106438</t>
+  </si>
+  <si>
+    <t>Jalem_11112</t>
+  </si>
+  <si>
+    <t>TC3:12</t>
+  </si>
+  <si>
+    <t>MJU6504106439</t>
+  </si>
+  <si>
+    <t>Pattara1_</t>
+  </si>
+  <si>
+    <t>TC3:13</t>
+  </si>
+  <si>
+    <t>MJU6504106440</t>
+  </si>
+  <si>
+    <t>Pattarawut_jam1</t>
+  </si>
+  <si>
+    <t>TC3:14</t>
+  </si>
+  <si>
+    <t>MJU6504106441</t>
+  </si>
+  <si>
+    <t>Pattarawut_kub11</t>
+  </si>
+  <si>
+    <t>TC3:15</t>
+  </si>
+  <si>
+    <t>MJU6504106442</t>
+  </si>
+  <si>
+    <t>1Jame##</t>
+  </si>
+  <si>
+    <t>รหัสผ่านต้องมีความยาวระหว่าง 8 - 16 ตัวอักษร</t>
+  </si>
+  <si>
+    <t>TC3:16</t>
+  </si>
+  <si>
+    <t>MJU6504106443</t>
+  </si>
+  <si>
+    <t>Pattarawut_123456</t>
+  </si>
+  <si>
+    <t>TC3:17</t>
+  </si>
+  <si>
+    <t>MJU6504106444</t>
+  </si>
+  <si>
+    <t>TC3:18</t>
+  </si>
+  <si>
+    <t>MJU6504106445</t>
+  </si>
+  <si>
+    <t>ptt_1234</t>
+  </si>
+  <si>
+    <t>รหัสผ่านต้องมีตัวพิมพ์ใหญ่ พิมพ์เล็ก และตัวเลข อย่างน้อย 1 ตัว</t>
+  </si>
+  <si>
     <t>Failed</t>
   </si>
   <si>
-    <t>TC3:02</t>
-  </si>
-  <si>
-    <t>pattrawut</t>
-  </si>
-  <si>
-    <t>กรุณากรอกข้อมูลอีเมล์ให้อยู่ในรูปแบบของ MJU เช่น (MJU6504106001@mju.ac.th)</t>
-  </si>
-  <si>
-    <t>ความยาวรหัสนักศึกษาต้องมี 13 ตัวพอดี</t>
-  </si>
-  <si>
-    <t>TC3:03</t>
-  </si>
-  <si>
-    <t>MJU6504106337</t>
-  </si>
-  <si>
-    <t>TC3:04</t>
-  </si>
-  <si>
-    <t>MJU 650410640</t>
-  </si>
-  <si>
-    <t>กรุณากรอกข้อมูลโดยห้ามมีช่องว่าง</t>
-  </si>
-  <si>
-    <t>กรุณากรอกข้อมูลอีเมล์และรหัสผ่านโดยห้ามมีช่องว่าง</t>
-  </si>
-  <si>
-    <t>TC3:05</t>
-  </si>
-  <si>
-    <t>mju6504106400</t>
-  </si>
-  <si>
-    <t>TC3:06</t>
-  </si>
-  <si>
-    <t>mju650410640</t>
-  </si>
-  <si>
-    <t>กรุณากรอกความยาวให้มีขนาด 13 ตัวพอดี</t>
-  </si>
-  <si>
-    <t>TC3:07</t>
-  </si>
-  <si>
-    <t>mju65041064001</t>
-  </si>
-  <si>
-    <t>TC3:08</t>
-  </si>
-  <si>
-    <t>กรุณากรอกอีเมล์รูปแบบของอีเมล MJU</t>
-  </si>
-  <si>
-    <t>กรุณากรอกรหัสนักศึกษาและรหัสผ่าน</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>TC3:09</t>
-  </si>
-  <si>
-    <t>MJU6504106436</t>
-  </si>
-  <si>
-    <t>TC3:10</t>
-  </si>
-  <si>
-    <t>MJU6504106437</t>
-  </si>
-  <si>
-    <t>รหัสผ่าน</t>
-  </si>
-  <si>
-    <t>กรุณากรอกประกอบด้วยตัวอักษรภาษาอังกฤษหรือตัวเลขรวมอักขระพิเศษ</t>
-  </si>
-  <si>
-    <t>ชื่อผู้ใช้หรือรหัสผ่านไม่ถูกต้อง</t>
-  </si>
-  <si>
-    <t>TC3:11</t>
-  </si>
-  <si>
-    <t>MJU6504106438</t>
-  </si>
-  <si>
-    <t>Jalem_11112</t>
-  </si>
-  <si>
-    <t>TC3:12</t>
-  </si>
-  <si>
-    <t>MJU6504106439</t>
-  </si>
-  <si>
-    <t>Pattara1_</t>
-  </si>
-  <si>
-    <t>TC3:13</t>
-  </si>
-  <si>
-    <t>MJU6504106440</t>
-  </si>
-  <si>
-    <t>Pattarawut_jam1</t>
-  </si>
-  <si>
-    <t>TC3:14</t>
-  </si>
-  <si>
-    <t>MJU6504106441</t>
-  </si>
-  <si>
-    <t>Pattarawut_kub11</t>
-  </si>
-  <si>
-    <t>TC3:15</t>
-  </si>
-  <si>
-    <t>MJU6504106442</t>
-  </si>
-  <si>
-    <t>1Jame##</t>
-  </si>
-  <si>
-    <t>กรุณากรอกได้ต้องแต่ 8 - 16 ตัวอักษร</t>
-  </si>
-  <si>
-    <t>รหัสผ่านต้องมีความยาวระหว่าง 8 - 16 ตัวอักษร</t>
-  </si>
-  <si>
-    <t>TC3:16</t>
-  </si>
-  <si>
-    <t>MJU6504106443</t>
-  </si>
-  <si>
-    <t>Pattarawut_123456</t>
-  </si>
-  <si>
-    <t>TC3:17</t>
-  </si>
-  <si>
-    <t>MJU6504106444</t>
-  </si>
-  <si>
-    <t>TC3:18</t>
-  </si>
-  <si>
-    <t>MJU650410645</t>
-  </si>
-  <si>
-    <t>ptt_1234</t>
-  </si>
-  <si>
-    <t>รหัสผ่านต้องมีตัวพิมพ์ใหญ่ พิมพ์เล็ก และตัวเลข อย่างน้อย 1 ตัว</t>
-  </si>
-  <si>
     <t>TC3:19</t>
   </si>
   <si>
@@ -247,16 +229,10 @@
     <t>Pattarawut# 1234</t>
   </si>
   <si>
-    <t>กรุณากรอกข้อมูลห้ามมีช่องว่างระหว่าตัวอักษร</t>
-  </si>
-  <si>
     <t>TC3:21</t>
   </si>
   <si>
     <t>MJU6504106448</t>
-  </si>
-  <si>
-    <t>กรุณากรอกรหัสผ่าน</t>
   </si>
 </sst>
 </file>
@@ -626,7 +602,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -634,10 +610,10 @@
     <col min="1" max="2" width="9.140625" style="3" customWidth="1"/>
     <col min="3" max="3" width="19" style="3" customWidth="1"/>
     <col min="4" max="4" width="14" style="3" customWidth="1"/>
-    <col min="5" max="5" width="49.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="53.140625" style="3" customWidth="1"/>
     <col min="6" max="6" width="47.140625" style="3" customWidth="1"/>
-    <col min="7" max="15" width="9.140625" style="3" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="3"/>
+    <col min="7" max="17" width="9.140625" style="3" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.5">
@@ -683,10 +659,10 @@
         <v>12</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" s="4"/>
     </row>
@@ -695,34 +671,34 @@
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>16</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>11</v>
@@ -731,46 +707,46 @@
         <v>12</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>11</v>
@@ -779,92 +755,92 @@
         <v>12</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>11</v>
@@ -873,190 +849,190 @@
         <v>12</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="E11" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>11</v>
@@ -1065,104 +1041,104 @@
         <v>12</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="4" t="s">
-        <v>78</v>
+        <v>30</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H22" s="4"/>
     </row>

</xml_diff>